<commit_message>
Paarweiser Vergleich und Berechnung mit Excel getestet
</commit_message>
<xml_diff>
--- a/RB-Blessing/Paarweiser_Vergleich.xlsx
+++ b/RB-Blessing/Paarweiser_Vergleich.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hopfm.tmb18\Documents\GitHub\KE3\RB-Blessing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\langohra.tmb18\Documents\GitHub\KE3\RB-Blessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A93307B-814A-41A9-848B-EE7EAEA583BA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ADD2C25-E963-4981-9338-E4540CF5AA14}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,32 +32,6 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Ein Microsoft Office-Anwender</author>
-    <author>Blessing</author>
-  </authors>
-  <commentList>
-    <comment ref="Y3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
-      <text/>
-    </comment>
-    <comment ref="Z3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
-      <text/>
-    </comment>
-    <comment ref="X8" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
-      <text/>
-    </comment>
-    <comment ref="Y14" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
-      <text/>
-    </comment>
-    <comment ref="Z17" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
-      <text/>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
@@ -79,19 +53,10 @@
     <t>lfd. Nr.</t>
   </si>
   <si>
-    <t>Anforderung 20</t>
-  </si>
-  <si>
     <t>Gewicht &lt; 15kg (Mechanik)</t>
   </si>
   <si>
     <t>Gleichartige Teile</t>
-  </si>
-  <si>
-    <t>Lebensdauer &lt; 100000h</t>
-  </si>
-  <si>
-    <t>Kompakt (Kettenlänge&lt;1000mm)</t>
   </si>
   <si>
     <t>Rostfreier Stahl</t>
@@ -121,12 +86,6 @@
     <t>Betrieb bei hohen Teperaturen (bis 40°C)</t>
   </si>
   <si>
-    <t>Niedriger Strom Verbrauch (&lt;4kWh)</t>
-  </si>
-  <si>
-    <t>Motorkraft hoch (&gt;2kW)</t>
-  </si>
-  <si>
     <t>Fettschmierung</t>
   </si>
   <si>
@@ -136,13 +95,28 @@
     <t>Getriebemotor</t>
   </si>
   <si>
-    <t>Automatik-Getriebe</t>
-  </si>
-  <si>
     <t>Antriebstrommellagerung eines Bandförderes</t>
   </si>
   <si>
     <t>Tanja Hofmann, Matthias Tiroch, Anika Langohr, Marie Hopf</t>
+  </si>
+  <si>
+    <t>Firmenlogo gut sichtbar angebracht</t>
+  </si>
+  <si>
+    <t>Motorleistung hoch (&gt;2kW)</t>
+  </si>
+  <si>
+    <t>Niedriger Stromverbrauch (&lt;4kWh)</t>
+  </si>
+  <si>
+    <t>Kompakt (Kettenlänge &lt; 1000mm)</t>
+  </si>
+  <si>
+    <t>Transportmaße unter 800mmx800mmx800mm</t>
+  </si>
+  <si>
+    <t>Lebensdauer &gt; 30000h</t>
   </si>
 </sst>
 </file>
@@ -152,7 +126,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="MS Sans Serif"/>
@@ -190,19 +164,6 @@
       <b/>
       <sz val="14"/>
       <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="81"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
@@ -711,7 +672,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1"/>
@@ -724,13 +685,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -746,15 +701,6 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -778,6 +724,21 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="6" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1306,14 +1267,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:AC112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB3" sqref="AB3"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1332,155 +1296,155 @@
   <sheetData>
     <row r="1" spans="2:29" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="32"/>
-      <c r="C1" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="36" t="s">
+      <c r="C1" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="37"/>
-      <c r="P1" s="37"/>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="37"/>
-      <c r="S1" s="37"/>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
       <c r="Z1" s="32"/>
     </row>
     <row r="2" spans="2:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="43"/>
-      <c r="D2" s="44" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45"/>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45"/>
-      <c r="W2" s="45"/>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="46"/>
-      <c r="Z2" s="43"/>
-    </row>
-    <row r="3" spans="2:29" ht="246" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39" t="s">
+      <c r="C2" s="41"/>
+      <c r="D2" s="52" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="53"/>
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="53"/>
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="41"/>
+    </row>
+    <row r="3" spans="2:29" ht="247.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="50" t="str">
+      <c r="C3" s="38"/>
+      <c r="D3" s="45" t="str">
         <f>$C4</f>
         <v>Gewicht &lt; 15kg (Mechanik)</v>
       </c>
-      <c r="E3" s="51" t="str">
+      <c r="E3" s="46" t="str">
         <f>$C5</f>
         <v>Gleichartige Teile</v>
       </c>
-      <c r="F3" s="51" t="str">
+      <c r="F3" s="46" t="str">
         <f>C6</f>
         <v>Günstig &lt; 800€</v>
       </c>
-      <c r="G3" s="51" t="str">
+      <c r="G3" s="46" t="str">
         <f>C7</f>
-        <v>Lebensdauer &lt; 100000h</v>
-      </c>
-      <c r="H3" s="51" t="str">
+        <v>Lebensdauer &gt; 30000h</v>
+      </c>
+      <c r="H3" s="46" t="str">
         <f>C8</f>
         <v>Getriebemotor</v>
       </c>
-      <c r="I3" s="51" t="str">
+      <c r="I3" s="46" t="str">
         <f>C9</f>
-        <v>Kompakt (Kettenlänge&lt;1000mm)</v>
-      </c>
-      <c r="J3" s="51" t="str">
+        <v>Kompakt (Kettenlänge &lt; 1000mm)</v>
+      </c>
+      <c r="J3" s="46" t="str">
         <f>C10</f>
         <v>Rostfreier Stahl</v>
       </c>
-      <c r="K3" s="51" t="str">
+      <c r="K3" s="46" t="str">
         <f>C11</f>
         <v>Netzbetrieb des Motors möglich</v>
       </c>
-      <c r="L3" s="51" t="str">
+      <c r="L3" s="46" t="str">
         <f>C12</f>
         <v>Magnetlagerung</v>
       </c>
-      <c r="M3" s="51" t="str">
+      <c r="M3" s="46" t="str">
         <f>C13</f>
         <v>Selbstzentrierendes Band</v>
       </c>
-      <c r="N3" s="51" t="str">
+      <c r="N3" s="46" t="str">
         <f>C14</f>
         <v>Im Freien benutzbar</v>
       </c>
-      <c r="O3" s="51" t="str">
+      <c r="O3" s="46" t="str">
         <f>C15</f>
         <v>Regelbare Geschwindigkeit</v>
       </c>
-      <c r="P3" s="51" t="str">
+      <c r="P3" s="46" t="str">
         <f>C16</f>
-        <v>Automatik-Getriebe</v>
-      </c>
-      <c r="Q3" s="51" t="str">
+        <v>Firmenlogo gut sichtbar angebracht</v>
+      </c>
+      <c r="Q3" s="46" t="str">
         <f>C17</f>
         <v>Betrieb bei niedrigen Teperaturen (bis -10°C)</v>
       </c>
-      <c r="R3" s="51" t="str">
+      <c r="R3" s="46" t="str">
         <f>C18</f>
         <v>Betrieb bei hohen Teperaturen (bis 40°C)</v>
       </c>
-      <c r="S3" s="51" t="str">
+      <c r="S3" s="46" t="str">
         <f>C19</f>
-        <v>Niedriger Strom Verbrauch (&lt;4kWh)</v>
-      </c>
-      <c r="T3" s="51" t="str">
+        <v>Niedriger Stromverbrauch (&lt;4kWh)</v>
+      </c>
+      <c r="T3" s="46" t="str">
         <f>C20</f>
-        <v>Motorkraft hoch (&gt;2kW)</v>
-      </c>
-      <c r="U3" s="51" t="str">
+        <v>Motorleistung hoch (&gt;2kW)</v>
+      </c>
+      <c r="U3" s="46" t="str">
         <f>C21</f>
         <v>Fettschmierung</v>
       </c>
-      <c r="V3" s="51" t="str">
+      <c r="V3" s="46" t="str">
         <f>C22</f>
         <v>Geräuscharm (&lt;70db)</v>
       </c>
-      <c r="W3" s="52" t="str">
+      <c r="W3" s="47" t="str">
         <f>C23</f>
-        <v>Anforderung 20</v>
-      </c>
-      <c r="X3" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="41" t="s">
+        <v>Transportmaße unter 800mmx800mmx800mm</v>
+      </c>
+      <c r="X3" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="Z3" s="42" t="s">
+      <c r="Z3" s="40" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1488,33 +1452,33 @@
       <c r="B4" s="33">
         <v>1</v>
       </c>
-      <c r="C4" s="47" t="s">
-        <v>7</v>
+      <c r="C4" s="42" t="s">
+        <v>6</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G4" s="4">
         <v>0</v>
       </c>
       <c r="H4" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I4" s="4">
         <v>0</v>
       </c>
       <c r="J4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="4">
         <v>0</v>
       </c>
       <c r="L4" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M4" s="4">
         <v>0</v>
@@ -1526,7 +1490,7 @@
         <v>0</v>
       </c>
       <c r="P4" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q4" s="5">
         <v>0</v>
@@ -1544,22 +1508,22 @@
         <v>0</v>
       </c>
       <c r="V4" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4" s="6">
         <v>0</v>
       </c>
       <c r="X4" s="7">
         <f t="shared" ref="X4:X23" si="0">SUM(IF(C4=0,0,SUM(D4:W4)))</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="Y4" s="31">
         <f>ROUND(X4/X$24*10,0)</f>
-        <v>0</v>
-      </c>
-      <c r="Z4" s="53">
+        <v>3</v>
+      </c>
+      <c r="Z4" s="48">
         <f>X4/$X$25*100</f>
-        <v>0</v>
+        <v>2.8947368421052633</v>
       </c>
       <c r="AB4" s="8"/>
     </row>
@@ -1567,12 +1531,12 @@
       <c r="B5" s="33">
         <v>2</v>
       </c>
-      <c r="C5" s="48" t="s">
-        <v>8</v>
+      <c r="C5" s="43" t="s">
+        <v>7</v>
       </c>
       <c r="D5" s="9">
         <f>2-E4</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="11">
@@ -1582,19 +1546,19 @@
         <v>0</v>
       </c>
       <c r="H5" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I5" s="11">
         <v>0</v>
       </c>
       <c r="J5" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="11">
         <v>0</v>
       </c>
       <c r="L5" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M5" s="11">
         <v>0</v>
@@ -1606,7 +1570,7 @@
         <v>0</v>
       </c>
       <c r="P5" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q5" s="12">
         <v>0</v>
@@ -1621,25 +1585,25 @@
         <v>0</v>
       </c>
       <c r="U5" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W5" s="13">
         <v>0</v>
       </c>
       <c r="X5" s="14">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="Y5" s="31">
         <f t="shared" ref="Y5:Y23" si="1">ROUND(X5/X$24*10,0)</f>
-        <v>1</v>
-      </c>
-      <c r="Z5" s="53">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="48">
         <f t="shared" ref="Z5:Z23" si="2">X5/$X$25*100</f>
-        <v>0.52631578947368418</v>
+        <v>2.6315789473684208</v>
       </c>
       <c r="AB5" s="15"/>
       <c r="AC5" s="16"/>
@@ -1648,12 +1612,12 @@
       <c r="B6" s="33">
         <v>3</v>
       </c>
-      <c r="C6" s="48" t="s">
-        <v>14</v>
+      <c r="C6" s="43" t="s">
+        <v>11</v>
       </c>
       <c r="D6" s="9">
         <f>2-F4</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E6" s="17">
         <f>2-F5</f>
@@ -1664,7 +1628,7 @@
         <v>0</v>
       </c>
       <c r="H6" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I6" s="11">
         <v>0</v>
@@ -1676,19 +1640,19 @@
         <v>0</v>
       </c>
       <c r="L6" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M6" s="11">
         <v>0</v>
       </c>
       <c r="N6" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P6" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q6" s="12">
         <v>0</v>
@@ -1697,31 +1661,31 @@
         <v>0</v>
       </c>
       <c r="S6" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T6" s="12">
         <v>0</v>
       </c>
       <c r="U6" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V6" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W6" s="13">
         <v>0</v>
       </c>
       <c r="X6" s="14">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="Y6" s="31">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="Z6" s="53">
+        <v>4</v>
+      </c>
+      <c r="Z6" s="48">
         <f t="shared" si="2"/>
-        <v>1.0526315789473684</v>
+        <v>3.9473684210526314</v>
       </c>
       <c r="AB6" s="15"/>
       <c r="AC6" s="16"/>
@@ -1730,8 +1694,8 @@
       <c r="B7" s="33">
         <v>4</v>
       </c>
-      <c r="C7" s="48" t="s">
-        <v>9</v>
+      <c r="C7" s="43" t="s">
+        <v>27</v>
       </c>
       <c r="D7" s="9">
         <f>2-G4</f>
@@ -1747,64 +1711,64 @@
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I7" s="11">
         <v>0</v>
       </c>
       <c r="J7" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="11">
         <v>0</v>
       </c>
       <c r="L7" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M7" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="11">
         <v>0</v>
       </c>
       <c r="O7" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P7" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q7" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R7" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S7" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T7" s="12">
         <v>0</v>
       </c>
       <c r="U7" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V7" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W7" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X7" s="14">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="Y7" s="31">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="Z7" s="53">
+        <v>8</v>
+      </c>
+      <c r="Z7" s="48">
         <f t="shared" si="2"/>
-        <v>1.5789473684210527</v>
+        <v>7.3684210526315779</v>
       </c>
       <c r="AB7" s="15"/>
       <c r="AC7" s="16"/>
@@ -1813,24 +1777,24 @@
       <c r="B8" s="33">
         <v>5</v>
       </c>
-      <c r="C8" s="48" t="s">
-        <v>24</v>
+      <c r="C8" s="43" t="s">
+        <v>19</v>
       </c>
       <c r="D8" s="9">
         <f>2-H4</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E8" s="17">
         <f>2-H5</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F8" s="17">
         <f>2-H6</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8" s="17">
         <f>2-H7</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="11">
@@ -1843,7 +1807,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M8" s="11">
         <v>0</v>
@@ -1855,7 +1819,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q8" s="12">
         <v>0</v>
@@ -1870,7 +1834,7 @@
         <v>0</v>
       </c>
       <c r="U8" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V8" s="12">
         <v>0</v>
@@ -1880,23 +1844,23 @@
       </c>
       <c r="X8" s="14">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="Y8" s="31">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="Z8" s="53">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="48">
         <f t="shared" si="2"/>
-        <v>2.1052631578947367</v>
+        <v>1.3157894736842104</v>
       </c>
     </row>
     <row r="9" spans="2:29" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="33">
         <v>6</v>
       </c>
-      <c r="C9" s="48" t="s">
-        <v>10</v>
+      <c r="C9" s="43" t="s">
+        <v>25</v>
       </c>
       <c r="D9" s="9">
         <f>2-I4</f>
@@ -1920,13 +1884,13 @@
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K9" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L9" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M9" s="11">
         <v>0</v>
@@ -1935,10 +1899,10 @@
         <v>0</v>
       </c>
       <c r="O9" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q9" s="12">
         <v>0</v>
@@ -1953,41 +1917,41 @@
         <v>0</v>
       </c>
       <c r="U9" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V9" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W9" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X9" s="14">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="Y9" s="31">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="Z9" s="53">
+        <v>6</v>
+      </c>
+      <c r="Z9" s="48">
         <f t="shared" si="2"/>
-        <v>2.6315789473684208</v>
+        <v>6.0526315789473681</v>
       </c>
     </row>
     <row r="10" spans="2:29" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="34">
         <v>7</v>
       </c>
-      <c r="C10" s="48" t="s">
-        <v>11</v>
+      <c r="C10" s="43" t="s">
+        <v>8</v>
       </c>
       <c r="D10" s="9">
         <f>2-J4</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" s="17">
         <f>2-J5</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F10" s="17">
         <f>2-J6</f>
@@ -1995,7 +1959,7 @@
       </c>
       <c r="G10" s="17">
         <f>2-J7</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H10" s="17">
         <f>2-J8</f>
@@ -2003,67 +1967,67 @@
       </c>
       <c r="I10" s="17">
         <f>2-J9</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="11">
         <v>0</v>
       </c>
       <c r="L10" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M10" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N10" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10" s="12">
         <v>0</v>
       </c>
       <c r="P10" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q10" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R10" s="12">
         <v>0</v>
       </c>
       <c r="S10" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10" s="12">
         <v>0</v>
       </c>
       <c r="U10" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V10" s="12">
         <v>0</v>
       </c>
       <c r="W10" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X10" s="14">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="Y10" s="31">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="Z10" s="53">
+        <v>6</v>
+      </c>
+      <c r="Z10" s="48">
         <f t="shared" si="2"/>
-        <v>3.1578947368421053</v>
+        <v>5.5263157894736841</v>
       </c>
     </row>
     <row r="11" spans="2:29" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="34">
         <v>8</v>
       </c>
-      <c r="C11" s="48" t="s">
-        <v>12</v>
+      <c r="C11" s="43" t="s">
+        <v>9</v>
       </c>
       <c r="D11" s="9">
         <f>2-K4</f>
@@ -2087,7 +2051,7 @@
       </c>
       <c r="I11" s="17">
         <f>2-K9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J11" s="17">
         <f>2-K10</f>
@@ -2095,22 +2059,22 @@
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M11" s="11">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N11" s="11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P11" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q11" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="12">
         <v>0</v>
@@ -2122,65 +2086,65 @@
         <v>0</v>
       </c>
       <c r="U11" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V11" s="12">
         <v>0</v>
       </c>
       <c r="W11" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X11" s="14">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="Y11" s="31">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="Z11" s="53">
+        <v>8</v>
+      </c>
+      <c r="Z11" s="48">
         <f t="shared" si="2"/>
-        <v>3.6842105263157889</v>
+        <v>7.1052631578947363</v>
       </c>
     </row>
     <row r="12" spans="2:29" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="34">
         <v>9</v>
       </c>
-      <c r="C12" s="48" t="s">
-        <v>13</v>
+      <c r="C12" s="43" t="s">
+        <v>10</v>
       </c>
       <c r="D12" s="9">
         <f>2-L4</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E12" s="17">
         <f>2-L5</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F12" s="17">
         <f>2-L6</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G12" s="17">
         <f>2-L7</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H12" s="17">
         <f>2-L8</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I12" s="17">
         <f>2-L9</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J12" s="17">
         <f>2-L10</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K12" s="17">
         <f>2-L11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L12" s="10"/>
       <c r="M12" s="11">
@@ -2218,23 +2182,23 @@
       </c>
       <c r="X12" s="14">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="31">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="Z12" s="53">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="48">
         <f t="shared" si="2"/>
-        <v>4.2105263157894735</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:29" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="34">
         <v>10</v>
       </c>
-      <c r="C13" s="48" t="s">
-        <v>15</v>
+      <c r="C13" s="43" t="s">
+        <v>12</v>
       </c>
       <c r="D13" s="9">
         <f>2-M4</f>
@@ -2250,7 +2214,7 @@
       </c>
       <c r="G13" s="17">
         <f>2-M7</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H13" s="17">
         <f>2-M8</f>
@@ -2262,11 +2226,11 @@
       </c>
       <c r="J13" s="17">
         <f>2-M10</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K13" s="17">
         <f>2-M11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L13" s="17">
         <f>2-M12</f>
@@ -2280,7 +2244,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q13" s="12">
         <v>0</v>
@@ -2295,33 +2259,33 @@
         <v>0</v>
       </c>
       <c r="U13" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V13" s="12">
         <v>0</v>
       </c>
       <c r="W13" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X13" s="14">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Y13" s="31">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="Z13" s="53">
+      <c r="Z13" s="48">
         <f t="shared" si="2"/>
-        <v>4.7368421052631584</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:29" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="34">
         <v>11</v>
       </c>
-      <c r="C14" s="48" t="s">
-        <v>16</v>
+      <c r="C14" s="43" t="s">
+        <v>13</v>
       </c>
       <c r="D14" s="9">
         <f>2-N4</f>
@@ -2333,7 +2297,7 @@
       </c>
       <c r="F14" s="17">
         <f>2-N6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14" s="17">
         <f>2-N7</f>
@@ -2349,11 +2313,11 @@
       </c>
       <c r="J14" s="17">
         <f>2-N10</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K14" s="17">
         <f>2-N11</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L14" s="17">
         <f>2-N12</f>
@@ -2365,10 +2329,10 @@
       </c>
       <c r="N14" s="10"/>
       <c r="O14" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="P14" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q14" s="18">
         <v>0</v>
@@ -2377,39 +2341,39 @@
         <v>0</v>
       </c>
       <c r="S14" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T14" s="18">
         <v>0</v>
       </c>
       <c r="U14" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V14" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W14" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X14" s="19">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="Y14" s="31">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="Z14" s="53">
+        <v>8</v>
+      </c>
+      <c r="Z14" s="48">
         <f t="shared" si="2"/>
-        <v>5.2631578947368416</v>
+        <v>7.3684210526315779</v>
       </c>
     </row>
     <row r="15" spans="2:29" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="34">
         <v>12</v>
       </c>
-      <c r="C15" s="48" t="s">
-        <v>17</v>
+      <c r="C15" s="43" t="s">
+        <v>14</v>
       </c>
       <c r="D15" s="9">
         <f>2-O$4</f>
@@ -2421,11 +2385,11 @@
       </c>
       <c r="F15" s="17">
         <f>2-O6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15" s="17">
         <f>2-O7</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H15" s="17">
         <f>2-O8</f>
@@ -2433,7 +2397,7 @@
       </c>
       <c r="I15" s="17">
         <f>2-O9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J15" s="17">
         <f>2-O10</f>
@@ -2441,7 +2405,7 @@
       </c>
       <c r="K15" s="17">
         <f>2-O11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L15" s="17">
         <f>2-O12</f>
@@ -2453,11 +2417,11 @@
       </c>
       <c r="N15" s="17">
         <f>2-O14</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O15" s="10"/>
       <c r="P15" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="18">
         <v>0</v>
@@ -2466,71 +2430,71 @@
         <v>0</v>
       </c>
       <c r="S15" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T15" s="18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U15" s="18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V15" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W15" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X15" s="19">
         <f t="shared" si="0"/>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="Y15" s="31">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="Z15" s="53">
+        <v>7</v>
+      </c>
+      <c r="Z15" s="48">
         <f t="shared" si="2"/>
-        <v>5.7894736842105265</v>
+        <v>6.5789473684210522</v>
       </c>
     </row>
     <row r="16" spans="2:29" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="34">
         <v>13</v>
       </c>
-      <c r="C16" s="48" t="s">
-        <v>25</v>
+      <c r="C16" s="43" t="s">
+        <v>22</v>
       </c>
       <c r="D16" s="9">
         <f>2-P4</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E16" s="17">
         <f>2-P5</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F16" s="17">
         <f>2-P6</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G16" s="17">
         <f>2-P7</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H16" s="17">
         <f>2-P8</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I16" s="17">
         <f>2-P9</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J16" s="17">
         <f>2-P10</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K16" s="17">
         <f>2-P11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L16" s="17">
         <f>2-P12</f>
@@ -2538,15 +2502,15 @@
       </c>
       <c r="M16" s="17">
         <f>2-P13</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N16" s="17">
         <f>2-P14</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O16" s="17">
         <f>2-P15</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="20">
@@ -2568,27 +2532,27 @@
         <v>0</v>
       </c>
       <c r="W16" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X16" s="19">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="Y16" s="31">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="Z16" s="53">
+        <v>1</v>
+      </c>
+      <c r="Z16" s="48">
         <f t="shared" si="2"/>
-        <v>6.3157894736842106</v>
+        <v>0.78947368421052633</v>
       </c>
     </row>
     <row r="17" spans="2:26" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="34">
         <v>14</v>
       </c>
-      <c r="C17" s="48" t="s">
-        <v>18</v>
+      <c r="C17" s="43" t="s">
+        <v>15</v>
       </c>
       <c r="D17" s="9">
         <f>2-Q4</f>
@@ -2604,7 +2568,7 @@
       </c>
       <c r="G17" s="17">
         <f>2-Q7</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H17" s="17">
         <f>2-Q8</f>
@@ -2616,11 +2580,11 @@
       </c>
       <c r="J17" s="17">
         <f>2-Q10</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K17" s="17">
         <f>2-Q11</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L17" s="17">
         <f>2-Q12</f>
@@ -2653,33 +2617,33 @@
         <v>0</v>
       </c>
       <c r="U17" s="20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V17" s="12">
         <v>0</v>
       </c>
       <c r="W17" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X17" s="19">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Y17" s="31">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="Z17" s="53">
+      <c r="Z17" s="48">
         <f t="shared" si="2"/>
-        <v>6.8421052631578956</v>
+        <v>6.3157894736842106</v>
       </c>
     </row>
     <row r="18" spans="2:26" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="34">
         <v>15</v>
       </c>
-      <c r="C18" s="48" t="s">
-        <v>19</v>
+      <c r="C18" s="43" t="s">
+        <v>16</v>
       </c>
       <c r="D18" s="9">
         <f>2-R4</f>
@@ -2695,7 +2659,7 @@
       </c>
       <c r="G18" s="17">
         <f>2-R7</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H18" s="17">
         <f>2-R8</f>
@@ -2739,39 +2703,39 @@
       </c>
       <c r="R18" s="10"/>
       <c r="S18" s="20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T18" s="20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U18" s="20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V18" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W18" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X18" s="19">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="Y18" s="31">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="Z18" s="53">
+        <v>10</v>
+      </c>
+      <c r="Z18" s="48">
         <f t="shared" si="2"/>
-        <v>7.3684210526315779</v>
+        <v>9.2105263157894726</v>
       </c>
     </row>
     <row r="19" spans="2:26" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="34">
         <v>16</v>
       </c>
-      <c r="C19" s="48" t="s">
-        <v>20</v>
+      <c r="C19" s="43" t="s">
+        <v>24</v>
       </c>
       <c r="D19" s="9">
         <f>2-S4</f>
@@ -2783,11 +2747,11 @@
       </c>
       <c r="F19" s="17">
         <f>2-S6</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19" s="17">
         <f>2-S7</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H19" s="17">
         <f>2-S8</f>
@@ -2799,7 +2763,7 @@
       </c>
       <c r="J19" s="17">
         <f>2-S10</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K19" s="17">
         <f>2-S11</f>
@@ -2815,11 +2779,11 @@
       </c>
       <c r="N19" s="17">
         <f>2-S14</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O19" s="17">
         <f>2-S15</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P19" s="17">
         <f>2-S16</f>
@@ -2831,40 +2795,40 @@
       </c>
       <c r="R19" s="17">
         <f>2-S18</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S19" s="10"/>
       <c r="T19" s="20">
         <v>0</v>
       </c>
       <c r="U19" s="20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V19" s="12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W19" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X19" s="19">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="Y19" s="31">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="Z19" s="53">
+        <v>7</v>
+      </c>
+      <c r="Z19" s="48">
         <f t="shared" si="2"/>
-        <v>7.8947368421052628</v>
+        <v>6.5789473684210522</v>
       </c>
     </row>
     <row r="20" spans="2:26" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="34">
         <v>17</v>
       </c>
-      <c r="C20" s="48" t="s">
-        <v>21</v>
+      <c r="C20" s="43" t="s">
+        <v>23</v>
       </c>
       <c r="D20" s="9">
         <f>2-T4</f>
@@ -2912,7 +2876,7 @@
       </c>
       <c r="O20" s="17">
         <f>2-T15</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P20" s="17">
         <f>2-T16</f>
@@ -2924,7 +2888,7 @@
       </c>
       <c r="R20" s="17">
         <f>2-T18</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S20" s="17">
         <f>2-T19</f>
@@ -2932,33 +2896,33 @@
       </c>
       <c r="T20" s="10"/>
       <c r="U20" s="20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V20" s="12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W20" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X20" s="19">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="Y20" s="31">
         <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="Z20" s="53">
+        <v>10</v>
+      </c>
+      <c r="Z20" s="48">
         <f t="shared" si="2"/>
-        <v>8.4210526315789469</v>
+        <v>9.4736842105263168</v>
       </c>
     </row>
     <row r="21" spans="2:26" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B21" s="34">
         <v>18</v>
       </c>
-      <c r="C21" s="48" t="s">
-        <v>22</v>
+      <c r="C21" s="43" t="s">
+        <v>17</v>
       </c>
       <c r="D21" s="9">
         <f>2-U4</f>
@@ -2966,31 +2930,31 @@
       </c>
       <c r="E21" s="17">
         <f>2-U5</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F21" s="17">
         <f>2-U6</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G21" s="17">
         <f>2-U7</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H21" s="17">
         <f>2-U8</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I21" s="17">
         <f>2-U9</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J21" s="17">
         <f>2-U10</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K21" s="17">
         <f>2-U11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L21" s="17">
         <f>2-U12</f>
@@ -2998,15 +2962,15 @@
       </c>
       <c r="M21" s="17">
         <f>2-U13</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N21" s="17">
         <f>2-U14</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O21" s="17">
         <f>2-U15</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P21" s="17">
         <f>2-U16</f>
@@ -3014,19 +2978,19 @@
       </c>
       <c r="Q21" s="17">
         <f>2-U17</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R21" s="17">
         <f>2-U18</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S21" s="17">
         <f>2-U19</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T21" s="17">
         <f>2-U20</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U21" s="10"/>
       <c r="V21" s="12">
@@ -3037,39 +3001,39 @@
       </c>
       <c r="X21" s="19">
         <f t="shared" si="0"/>
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="Y21" s="31">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="Z21" s="53">
+        <v>2</v>
+      </c>
+      <c r="Z21" s="48">
         <f t="shared" si="2"/>
-        <v>8.9473684210526319</v>
+        <v>2.1052631578947367</v>
       </c>
     </row>
     <row r="22" spans="2:26" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B22" s="34">
         <v>19</v>
       </c>
-      <c r="C22" s="48" t="s">
-        <v>23</v>
+      <c r="C22" s="43" t="s">
+        <v>18</v>
       </c>
       <c r="D22" s="9">
         <f>2-V4</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="17">
         <f>2-V5</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" s="17">
         <f>2-V6</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G22" s="17">
         <f>2-V7</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H22" s="17">
         <f>2-V8</f>
@@ -3077,7 +3041,7 @@
       </c>
       <c r="I22" s="17">
         <f>2-V9</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J22" s="17">
         <f>2-V10</f>
@@ -3097,11 +3061,11 @@
       </c>
       <c r="N22" s="17">
         <f>2-V14</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O22" s="17">
         <f>2-V15</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P22" s="17">
         <f>2-V16</f>
@@ -3113,15 +3077,15 @@
       </c>
       <c r="R22" s="17">
         <f>2-V18</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S22" s="17">
         <f>2-V19</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T22" s="17">
         <f>2-V20</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U22" s="17">
         <f>2-V21</f>
@@ -3129,27 +3093,27 @@
       </c>
       <c r="V22" s="10"/>
       <c r="W22" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X22" s="19">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="Y22" s="31">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="Z22" s="53">
+        <v>6</v>
+      </c>
+      <c r="Z22" s="48">
         <f t="shared" si="2"/>
-        <v>9.4736842105263168</v>
+        <v>5.5263157894736841</v>
       </c>
     </row>
     <row r="23" spans="2:26" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="35">
         <v>20</v>
       </c>
-      <c r="C23" s="49" t="s">
-        <v>6</v>
+      <c r="C23" s="44" t="s">
+        <v>26</v>
       </c>
       <c r="D23" s="21">
         <f>2-W4</f>
@@ -3165,7 +3129,7 @@
       </c>
       <c r="G23" s="22">
         <f>2-W7</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H23" s="22">
         <f>2-W8</f>
@@ -3173,15 +3137,15 @@
       </c>
       <c r="I23" s="22">
         <f>2-W9</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J23" s="22">
         <f>2-W10</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K23" s="22">
         <f>2-W11</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L23" s="22">
         <f>2-W12</f>
@@ -3189,35 +3153,35 @@
       </c>
       <c r="M23" s="22">
         <f>2-W13</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N23" s="22">
         <f>2-W14</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="O23" s="22">
         <f>2-W15</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="P23" s="22">
         <f>2-W16</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q23" s="22">
         <f>2-W17</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R23" s="22">
         <f>2-W18</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S23" s="22">
         <f>2-W19</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T23" s="22">
         <f>2-W20</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="U23" s="22">
         <f>2-W21</f>
@@ -3225,20 +3189,20 @@
       </c>
       <c r="V23" s="22">
         <f>2-W22</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W23" s="23"/>
       <c r="X23" s="24">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="Y23" s="31">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="Z23" s="54">
+        <v>4</v>
+      </c>
+      <c r="Z23" s="49">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>4.2105263157894735</v>
       </c>
     </row>
     <row r="24" spans="2:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3267,12 +3231,12 @@
       </c>
       <c r="X24" s="2">
         <f>MAX(X4:X23)</f>
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Y24" s="27"/>
       <c r="Z24" s="2">
         <f>MAX(Z4:Z23)</f>
-        <v>10</v>
+        <v>9.4736842105263168</v>
       </c>
     </row>
     <row r="25" spans="2:26" x14ac:dyDescent="0.2">
@@ -3306,7 +3270,7 @@
       <c r="Y25" s="27"/>
       <c r="Z25" s="2">
         <f>SUM(Z4:Z23)</f>
-        <v>100</v>
+        <v>100.00000000000001</v>
       </c>
     </row>
     <row r="26" spans="2:26" x14ac:dyDescent="0.2">
@@ -5361,6 +5325,5 @@
     <oddFooter>&amp;L&amp;"Futura Light,Regular"Erstellung: TQU/DE &amp;D&amp;R&amp;"Futura Light,Regular"Datei: &amp;F&amp;A</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>